<commit_message>
Find the university which has changed namees
</commit_message>
<xml_diff>
--- a/ScienceAdmissionScore.xlsx
+++ b/ScienceAdmissionScore.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="380">
   <si>
     <t>院校号</t>
   </si>
@@ -1035,9 +1035,6 @@
   </si>
   <si>
     <t>10570</t>
-  </si>
-  <si>
-    <t>广州医学院</t>
   </si>
   <si>
     <t>10572</t>
@@ -3597,7 +3594,7 @@
   <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6212,7 +6209,7 @@
         <v>264</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>265</v>
+        <v>333</v>
       </c>
       <c r="C131" s="2">
         <v>408</v>
@@ -6229,10 +6226,10 @@
     </row>
     <row r="132" spans="1:6" ht="15">
       <c r="A132" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="C132" s="2">
         <v>1808</v>
@@ -6249,10 +6246,10 @@
     </row>
     <row r="133" spans="1:6" ht="15">
       <c r="A133" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B133" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="C133" s="2">
         <v>1693</v>
@@ -6269,10 +6266,10 @@
     </row>
     <row r="134" spans="1:6" ht="15">
       <c r="A134" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B134" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>271</v>
       </c>
       <c r="C134" s="2">
         <v>5457</v>
@@ -6289,10 +6286,10 @@
     </row>
     <row r="135" spans="1:6" ht="15">
       <c r="A135" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B135" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="C135" s="2">
         <v>15</v>
@@ -6307,10 +6304,10 @@
     </row>
     <row r="136" spans="1:6" ht="15">
       <c r="A136" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B136" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="C136" s="2">
         <v>16</v>
@@ -6325,10 +6322,10 @@
     </row>
     <row r="137" spans="1:6" ht="15">
       <c r="A137" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B137" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="C137" s="2">
         <v>11</v>
@@ -6343,10 +6340,10 @@
     </row>
     <row r="138" spans="1:6" ht="15">
       <c r="A138" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B138" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="C138" s="2">
         <v>20</v>
@@ -6361,10 +6358,10 @@
     </row>
     <row r="139" spans="1:6" ht="15">
       <c r="A139" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="C139" s="2">
         <v>6</v>
@@ -6387,8 +6384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" activeCellId="1" sqref="F108 G14"/>
+    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6400,7 +6397,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -6643,7 +6640,7 @@
         <v>19248</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C13" s="4">
         <v>8</v>
@@ -7783,7 +7780,7 @@
         <v>10276</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C70" s="4">
         <v>27</v>
@@ -8143,7 +8140,7 @@
         <v>19213</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C88" s="4">
         <v>20</v>
@@ -8303,7 +8300,7 @@
         <v>10570</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>265</v>
+        <v>333</v>
       </c>
       <c r="C96" s="4">
         <v>310</v>
@@ -8461,7 +8458,7 @@
         <v>10043</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C104" s="4">
         <v>14</v>
@@ -8515,7 +8512,7 @@
         <v>10126</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C107" s="4">
         <v>7</v>
@@ -8585,7 +8582,7 @@
         <v>10184</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C111" s="4">
         <v>6</v>
@@ -8637,7 +8634,7 @@
         <v>10225</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C114" s="4">
         <v>19</v>
@@ -8887,7 +8884,7 @@
         <v>10564</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C128" s="4">
         <v>5324</v>
@@ -8905,7 +8902,7 @@
         <v>10572</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C129" s="4">
         <v>1807</v>
@@ -9013,7 +9010,7 @@
         <v>10700</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C135" s="4">
         <v>54</v>
@@ -9101,7 +9098,7 @@
         <v>12121</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C140" s="4">
         <v>1899</v>
@@ -9155,7 +9152,7 @@
         <v>19614</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C143" s="4">
         <v>20</v>
@@ -9178,8 +9175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F176" sqref="F176:F187"/>
+    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9189,7 +9186,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -9392,7 +9389,7 @@
         <v>19248</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" s="5">
         <v>8</v>
@@ -9552,7 +9549,7 @@
         <v>19002</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -9892,7 +9889,7 @@
         <v>10054</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C36" s="5">
         <v>72</v>
@@ -10372,7 +10369,7 @@
         <v>19013</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C60" s="5">
         <v>19</v>
@@ -10412,7 +10409,7 @@
         <v>10079</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C62" s="5">
         <v>67</v>
@@ -10472,7 +10469,7 @@
         <v>19213</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C65" s="5">
         <v>25</v>
@@ -10492,7 +10489,7 @@
         <v>10276</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C66" s="5">
         <v>27</v>
@@ -10692,7 +10689,7 @@
         <v>10491</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C76" s="5">
         <v>47</v>
@@ -10752,7 +10749,7 @@
         <v>10425</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C79" s="5">
         <v>40</v>
@@ -10832,7 +10829,7 @@
         <v>11415</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C83" s="5">
         <v>29</v>
@@ -10872,7 +10869,7 @@
         <v>10570</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>265</v>
+        <v>333</v>
       </c>
       <c r="C85" s="5">
         <v>208</v>
@@ -10932,7 +10929,7 @@
         <v>10269</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C88" s="5">
         <v>12</v>
@@ -11052,7 +11049,7 @@
         <v>10366</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C94" s="5">
         <v>3</v>
@@ -11092,7 +11089,7 @@
         <v>19614</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C96" s="5">
         <v>20</v>
@@ -11172,7 +11169,7 @@
         <v>11413</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C100" s="5">
         <v>7</v>
@@ -11332,7 +11329,7 @@
         <v>10043</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C108" s="5">
         <v>11</v>
@@ -11386,7 +11383,7 @@
         <v>10126</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C111" s="5">
         <v>6</v>
@@ -11436,7 +11433,7 @@
         <v>10184</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C114" s="5">
         <v>6</v>
@@ -11504,7 +11501,7 @@
         <v>10225</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C118" s="5">
         <v>23</v>
@@ -11736,7 +11733,7 @@
         <v>10564</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C131" s="5">
         <v>5259</v>
@@ -11754,7 +11751,7 @@
         <v>10572</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C132" s="5">
         <v>1462</v>
@@ -11862,7 +11859,7 @@
         <v>10700</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C138" s="5">
         <v>42</v>
@@ -11932,7 +11929,7 @@
         <v>10755</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C142" s="5">
         <v>4</v>
@@ -11948,7 +11945,7 @@
         <v>11414</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C143" s="5">
         <v>16</v>
@@ -11966,7 +11963,7 @@
         <v>12121</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C144" s="5">
         <v>1500</v>
@@ -12002,7 +11999,7 @@
         <v>19359</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C146" s="5">
         <v>64</v>
@@ -12040,7 +12037,7 @@
         <v>10254</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C148" s="7">
         <v>127</v>
@@ -12060,7 +12057,7 @@
         <v>10700</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C149" s="7">
         <v>36</v>
@@ -12120,7 +12117,7 @@
         <v>10490</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C152" s="7">
         <v>34</v>
@@ -12158,7 +12155,7 @@
         <v>10110</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C154" s="7">
         <v>94</v>
@@ -12176,7 +12173,7 @@
         <v>10126</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C155" s="7">
         <v>41</v>
@@ -12212,7 +12209,7 @@
         <v>10184</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C157" s="7">
         <v>8</v>
@@ -12230,7 +12227,7 @@
         <v>10186</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C158" s="7">
         <v>150</v>
@@ -12248,7 +12245,7 @@
         <v>10212</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C159" s="7">
         <v>61</v>
@@ -12264,7 +12261,7 @@
         <v>10214</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C160" s="7">
         <v>121</v>
@@ -12316,7 +12313,7 @@
         <v>10224</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C163" s="7">
         <v>24</v>
@@ -12334,7 +12331,7 @@
         <v>10225</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C164" s="7">
         <v>24</v>
@@ -12352,7 +12349,7 @@
         <v>10264</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C165" s="7">
         <v>81</v>
@@ -12370,7 +12367,7 @@
         <v>10298</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C166" s="7">
         <v>80</v>
@@ -12388,7 +12385,7 @@
         <v>10366</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C167" s="7">
         <v>8</v>
@@ -12406,7 +12403,7 @@
         <v>10394</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C168" s="7">
         <v>52</v>
@@ -12424,7 +12421,7 @@
         <v>10404</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C169" s="7">
         <v>59</v>
@@ -12442,7 +12439,7 @@
         <v>10407</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C170" s="7">
         <v>100</v>
@@ -12460,7 +12457,7 @@
         <v>10427</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C171" s="7">
         <v>100</v>
@@ -12478,7 +12475,7 @@
         <v>10475</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C172" s="7">
         <v>94</v>
@@ -12496,7 +12493,7 @@
         <v>10534</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C173" s="7">
         <v>72</v>
@@ -12514,7 +12511,7 @@
         <v>10536</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C174" s="7">
         <v>161</v>
@@ -12532,7 +12529,7 @@
         <v>10537</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C175" s="7">
         <v>130</v>
@@ -12550,7 +12547,7 @@
         <v>10538</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C176" s="7">
         <v>94</v>
@@ -12568,7 +12565,7 @@
         <v>10555</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C177" s="7">
         <v>180</v>
@@ -12586,7 +12583,7 @@
         <v>10566</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C178" s="7">
         <v>1311</v>
@@ -12604,7 +12601,7 @@
         <v>10571</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C179" s="7">
         <v>688</v>
@@ -12622,7 +12619,7 @@
         <v>10572</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C180" s="7">
         <v>1299</v>
@@ -12640,7 +12637,7 @@
         <v>10616</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C181" s="7">
         <v>64</v>
@@ -12658,7 +12655,7 @@
         <v>10626</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C182" s="7">
         <v>10</v>
@@ -12694,7 +12691,7 @@
         <v>11414</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C184" s="7">
         <v>19</v>
@@ -12712,7 +12709,7 @@
         <v>19635</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C185" s="7">
         <v>48</v>
@@ -12730,7 +12727,7 @@
         <v>60145</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C186" s="7">
         <v>15</v>
@@ -12748,7 +12745,7 @@
         <v>60173</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C187" s="7">
         <v>10</v>
@@ -12771,8 +12768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12782,7 +12779,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5">
       <c r="A1" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
@@ -12797,7 +12794,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
@@ -12905,7 +12902,7 @@
         <v>19248</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7" s="12">
         <v>8</v>
@@ -12945,7 +12942,7 @@
         <v>19246</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" s="12">
         <v>15</v>
@@ -13085,7 +13082,7 @@
         <v>19002</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C16" s="12">
         <v>6</v>
@@ -13525,7 +13522,7 @@
         <v>10269</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C38" s="12">
         <v>20</v>
@@ -13825,7 +13822,7 @@
         <v>19213</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C53" s="12">
         <v>30</v>
@@ -13885,7 +13882,7 @@
         <v>11846</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C56" s="12">
         <v>1821</v>
@@ -14125,7 +14122,7 @@
         <v>10276</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C68" s="12">
         <v>34</v>
@@ -14185,7 +14182,7 @@
         <v>19614</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C71" s="12">
         <v>30</v>
@@ -14245,7 +14242,7 @@
         <v>10366</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C74" s="12">
         <v>8</v>
@@ -14305,7 +14302,7 @@
         <v>10590</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C77" s="12">
         <v>620</v>
@@ -14525,7 +14522,7 @@
         <v>12121</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C88" s="12">
         <v>1262</v>
@@ -14765,7 +14762,7 @@
         <v>10570</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C100" s="12">
         <v>441</v>
@@ -15005,7 +15002,7 @@
         <v>10343</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C112" s="12">
         <v>15</v>
@@ -15065,7 +15062,7 @@
         <v>10043</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C115" s="12">
         <v>16</v>
@@ -15155,7 +15152,7 @@
         <v>10126</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C120" s="12">
         <v>7</v>
@@ -15223,7 +15220,7 @@
         <v>10184</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C124" s="12">
         <v>6</v>
@@ -15277,7 +15274,7 @@
         <v>10224</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C127" s="12">
         <v>79</v>
@@ -15295,7 +15292,7 @@
         <v>10225</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C128" s="12">
         <v>26</v>
@@ -15473,7 +15470,7 @@
         <v>10564</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C138" s="12">
         <v>5622</v>
@@ -15491,7 +15488,7 @@
         <v>10572</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C139" s="12">
         <v>1322</v>
@@ -15545,7 +15542,7 @@
         <v>10626</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C142" s="12">
         <v>20</v>
@@ -15579,7 +15576,7 @@
         <v>10700</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C144" s="12">
         <v>45</v>
@@ -15649,7 +15646,7 @@
         <v>10755</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C148" s="12">
         <v>4</v>
@@ -15665,7 +15662,7 @@
         <v>11078</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C149" s="12">
         <v>767</v>
@@ -15683,7 +15680,7 @@
         <v>11845</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C150" s="12">
         <v>4949</v>
@@ -15701,7 +15698,7 @@
         <v>19141</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C151" s="12">
         <v>13</v>
@@ -15737,7 +15734,7 @@
         <v>19359</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C153" s="12">
         <v>80</v>
@@ -15760,8 +15757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15771,7 +15768,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -15974,7 +15971,7 @@
         <v>19246</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C11" s="15">
         <v>11</v>
@@ -16074,7 +16071,7 @@
         <v>19248</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C16" s="15">
         <v>7</v>
@@ -16254,7 +16251,7 @@
         <v>10269</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="15">
         <v>18</v>
@@ -16654,7 +16651,7 @@
         <v>80001</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C45" s="15">
         <v>242</v>
@@ -16794,7 +16791,7 @@
         <v>19614</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C52" s="15">
         <v>55</v>
@@ -16834,7 +16831,7 @@
         <v>19213</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C54" s="15">
         <v>35</v>
@@ -16854,7 +16851,7 @@
         <v>10276</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C55" s="15">
         <v>30</v>
@@ -16894,7 +16891,7 @@
         <v>10590</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C57" s="15">
         <v>1211</v>
@@ -16934,7 +16931,7 @@
         <v>11414</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C59" s="15">
         <v>17</v>
@@ -17094,7 +17091,7 @@
         <v>19013</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C67" s="15">
         <v>26</v>
@@ -17114,7 +17111,7 @@
         <v>12121</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C68" s="15">
         <v>1128</v>
@@ -17254,7 +17251,7 @@
         <v>10054</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C75" s="15">
         <v>86</v>
@@ -17274,7 +17271,7 @@
         <v>60384</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C76" s="15">
         <v>12</v>
@@ -17394,7 +17391,7 @@
         <v>11415</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C82" s="15">
         <v>35</v>
@@ -17434,7 +17431,7 @@
         <v>60652</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C84" s="15">
         <v>4</v>
@@ -17454,7 +17451,7 @@
         <v>11413</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C85" s="15">
         <v>17</v>
@@ -17494,7 +17491,7 @@
         <v>10343</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C87" s="15">
         <v>15</v>
@@ -17514,7 +17511,7 @@
         <v>10366</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C88" s="15">
         <v>8</v>
@@ -17534,7 +17531,7 @@
         <v>10491</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C89" s="15">
         <v>84</v>
@@ -17594,7 +17591,7 @@
         <v>10319</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C92" s="15">
         <v>2</v>
@@ -17734,7 +17731,7 @@
         <v>10421</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C99" s="15">
         <v>93</v>
@@ -17754,7 +17751,7 @@
         <v>10425</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C100" s="15">
         <v>55</v>
@@ -17774,7 +17771,7 @@
         <v>10043</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C101" s="15">
         <v>6</v>
@@ -17914,7 +17911,7 @@
         <v>19141</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C108" s="15">
         <v>14</v>
@@ -18034,7 +18031,7 @@
         <v>11078</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C114" s="15">
         <v>1183</v>
@@ -18054,7 +18051,7 @@
         <v>10570</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C115" s="15">
         <v>1129</v>
@@ -18194,7 +18191,7 @@
         <v>11845</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C122" s="15">
         <v>7340</v>
@@ -18214,7 +18211,7 @@
         <v>10564</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C123" s="15">
         <v>4754</v>
@@ -18324,7 +18321,7 @@
         <v>10079</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C129" s="15">
         <v>80</v>
@@ -18378,7 +18375,7 @@
         <v>10126</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C132" s="15">
         <v>6</v>
@@ -18482,7 +18479,7 @@
         <v>10184</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C138" s="15">
         <v>6</v>
@@ -18532,7 +18529,7 @@
         <v>10224</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C141" s="15">
         <v>34</v>
@@ -18548,7 +18545,7 @@
         <v>10225</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C142" s="15">
         <v>16</v>
@@ -18584,7 +18581,7 @@
         <v>10254</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C144" s="15">
         <v>134</v>
@@ -18602,7 +18599,7 @@
         <v>10264</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C145" s="15">
         <v>81</v>
@@ -18674,7 +18671,7 @@
         <v>10338</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C149" s="15">
         <v>130</v>
@@ -18692,7 +18689,7 @@
         <v>10490</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C150" s="15">
         <v>30</v>
@@ -18710,7 +18707,7 @@
         <v>10537</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C151" s="15">
         <v>101</v>
@@ -18726,7 +18723,7 @@
         <v>10538</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C152" s="15">
         <v>94</v>
@@ -18742,7 +18739,7 @@
         <v>10555</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C153" s="15">
         <v>100</v>
@@ -18760,7 +18757,7 @@
         <v>10572</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C154" s="15">
         <v>1214</v>
@@ -18796,7 +18793,7 @@
         <v>10626</v>
       </c>
       <c r="B156" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C156" s="15">
         <v>10</v>
@@ -18814,7 +18811,7 @@
         <v>10700</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C157" s="15">
         <v>36</v>
@@ -18884,7 +18881,7 @@
         <v>10755</v>
       </c>
       <c r="B161" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C161" s="15">
         <v>2</v>
@@ -18900,7 +18897,7 @@
         <v>19002</v>
       </c>
       <c r="B162" s="16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C162" s="15">
         <v>10</v>
@@ -18936,7 +18933,7 @@
         <v>19359</v>
       </c>
       <c r="B164" s="16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C164" s="15">
         <v>64</v>
@@ -18959,8 +18956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18970,7 +18967,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>1</v>
@@ -18979,7 +18976,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>4</v>
@@ -19073,7 +19070,7 @@
         <v>19248</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -19093,7 +19090,7 @@
         <v>19246</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
@@ -19313,7 +19310,7 @@
         <v>10027</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C18" s="7">
         <v>20</v>
@@ -19393,7 +19390,7 @@
         <v>19002</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C22" s="7">
         <v>10</v>
@@ -19433,7 +19430,7 @@
         <v>10269</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C24" s="7">
         <v>25</v>
@@ -19473,7 +19470,7 @@
         <v>19335</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C26" s="7">
         <v>20</v>
@@ -20033,7 +20030,7 @@
         <v>10276</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C54" s="7">
         <v>16</v>
@@ -20093,7 +20090,7 @@
         <v>19614</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C57" s="7">
         <v>55</v>
@@ -20133,7 +20130,7 @@
         <v>60384</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C59" s="7">
         <v>16</v>
@@ -20193,7 +20190,7 @@
         <v>10054</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C62" s="7">
         <v>87</v>
@@ -20273,7 +20270,7 @@
         <v>10590</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C66" s="7">
         <v>2017</v>
@@ -20293,7 +20290,7 @@
         <v>19213</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C67" s="7">
         <v>42</v>
@@ -20313,7 +20310,7 @@
         <v>60652</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C68" s="7">
         <v>4</v>
@@ -20553,7 +20550,7 @@
         <v>19013</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C80" s="7">
         <v>28</v>
@@ -20733,7 +20730,7 @@
         <v>60651</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C89" s="7">
         <v>8</v>
@@ -20753,7 +20750,7 @@
         <v>60033</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C90" s="7">
         <v>7</v>
@@ -20773,7 +20770,7 @@
         <v>10421</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C91" s="7">
         <v>90</v>
@@ -20813,7 +20810,7 @@
         <v>80001</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C93" s="7">
         <v>240</v>
@@ -20873,7 +20870,7 @@
         <v>10079</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C96" s="7">
         <v>82</v>
@@ -21053,7 +21050,7 @@
         <v>11415</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C105" s="7">
         <v>36</v>
@@ -21113,7 +21110,7 @@
         <v>10491</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C108" s="7">
         <v>88</v>
@@ -21133,7 +21130,7 @@
         <v>10319</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C109" s="7">
         <v>5</v>
@@ -21213,7 +21210,7 @@
         <v>12121</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C113" s="7">
         <v>1522</v>
@@ -21253,7 +21250,7 @@
         <v>10760</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C115" s="7">
         <v>1</v>
@@ -21333,7 +21330,7 @@
         <v>10425</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C119" s="7">
         <v>60</v>
@@ -21353,7 +21350,7 @@
         <v>19141</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C120" s="7">
         <v>15</v>
@@ -21473,7 +21470,7 @@
         <v>10570</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C126" s="7">
         <v>1288</v>
@@ -21513,7 +21510,7 @@
         <v>10343</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C128" s="7">
         <v>16</v>
@@ -21613,7 +21610,7 @@
         <v>11413</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C133" s="7">
         <v>20</v>
@@ -21673,7 +21670,7 @@
         <v>11078</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C136" s="7">
         <v>3228</v>
@@ -21693,7 +21690,7 @@
         <v>11845</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C137" s="7">
         <v>6792</v>
@@ -21713,7 +21710,7 @@
         <v>10043</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C138" s="7">
         <v>12</v>
@@ -21733,7 +21730,7 @@
         <v>10338</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C139" s="7">
         <v>130</v>
@@ -21753,7 +21750,7 @@
         <v>10564</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C140" s="7">
         <v>4996</v>
@@ -21793,7 +21790,7 @@
         <v>89012</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C142" s="7">
         <v>20</v>
@@ -21873,7 +21870,7 @@
         <v>19359</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C146" s="7">
         <v>64</v>
@@ -21913,7 +21910,7 @@
         <v>10254</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C148" s="7">
         <v>127</v>
@@ -21933,7 +21930,7 @@
         <v>10700</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C149" s="7">
         <v>36</v>
@@ -21993,7 +21990,7 @@
         <v>10490</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C152" s="7">
         <v>34</v>
@@ -22031,7 +22028,7 @@
         <v>10110</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C154" s="7">
         <v>94</v>
@@ -22049,7 +22046,7 @@
         <v>10126</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C155" s="7">
         <v>41</v>
@@ -22085,7 +22082,7 @@
         <v>10184</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C157" s="7">
         <v>8</v>
@@ -22103,7 +22100,7 @@
         <v>10186</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C158" s="7">
         <v>150</v>
@@ -22121,7 +22118,7 @@
         <v>10212</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C159" s="7">
         <v>61</v>
@@ -22137,7 +22134,7 @@
         <v>10214</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C160" s="7">
         <v>121</v>
@@ -22189,7 +22186,7 @@
         <v>10224</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C163" s="7">
         <v>24</v>
@@ -22207,7 +22204,7 @@
         <v>10225</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C164" s="7">
         <v>24</v>
@@ -22225,7 +22222,7 @@
         <v>10264</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C165" s="7">
         <v>81</v>
@@ -22243,7 +22240,7 @@
         <v>10298</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C166" s="7">
         <v>80</v>
@@ -22261,7 +22258,7 @@
         <v>10366</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C167" s="7">
         <v>8</v>
@@ -22279,7 +22276,7 @@
         <v>10394</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C168" s="7">
         <v>52</v>
@@ -22297,7 +22294,7 @@
         <v>10404</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C169" s="7">
         <v>59</v>
@@ -22315,7 +22312,7 @@
         <v>10407</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C170" s="7">
         <v>100</v>
@@ -22333,7 +22330,7 @@
         <v>10427</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C171" s="7">
         <v>100</v>
@@ -22351,7 +22348,7 @@
         <v>10475</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C172" s="7">
         <v>94</v>
@@ -22369,7 +22366,7 @@
         <v>10534</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C173" s="7">
         <v>72</v>
@@ -22387,7 +22384,7 @@
         <v>10536</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C174" s="7">
         <v>161</v>
@@ -22405,7 +22402,7 @@
         <v>10537</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C175" s="7">
         <v>130</v>
@@ -22423,7 +22420,7 @@
         <v>10538</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C176" s="7">
         <v>94</v>
@@ -22441,7 +22438,7 @@
         <v>10555</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C177" s="7">
         <v>180</v>
@@ -22459,7 +22456,7 @@
         <v>10566</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C178" s="7">
         <v>1311</v>
@@ -22477,7 +22474,7 @@
         <v>10571</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C179" s="7">
         <v>688</v>
@@ -22495,7 +22492,7 @@
         <v>10572</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C180" s="7">
         <v>1299</v>
@@ -22513,7 +22510,7 @@
         <v>10616</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C181" s="7">
         <v>64</v>
@@ -22531,7 +22528,7 @@
         <v>10626</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C182" s="7">
         <v>10</v>
@@ -22567,7 +22564,7 @@
         <v>11414</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C184" s="7">
         <v>19</v>
@@ -22585,7 +22582,7 @@
         <v>19635</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C185" s="7">
         <v>48</v>
@@ -22603,7 +22600,7 @@
         <v>60145</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C186" s="7">
         <v>15</v>
@@ -22621,7 +22618,7 @@
         <v>60173</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C187" s="7">
         <v>10</v>

</xml_diff>

<commit_message>
Insert the last ranking into the NaN data
</commit_message>
<xml_diff>
--- a/ScienceAdmissionScore.xlsx
+++ b/ScienceAdmissionScore.xlsx
@@ -19,12 +19,12 @@
     <sheet name="2014" sheetId="5" r:id="rId5"/>
     <sheet name="2015" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="380">
   <si>
     <t>院校号</t>
   </si>
@@ -3593,8 +3593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F139" sqref="F139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6300,7 +6300,9 @@
       <c r="E135" s="2">
         <v>621</v>
       </c>
-      <c r="F135" s="2"/>
+      <c r="F135" s="2">
+        <v>29550</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="15">
       <c r="A136" s="2" t="s">
@@ -6318,7 +6320,9 @@
       <c r="E136" s="2">
         <v>621</v>
       </c>
-      <c r="F136" s="2"/>
+      <c r="F136" s="2">
+        <v>29550</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="15">
       <c r="A137" s="2" t="s">
@@ -6336,7 +6340,9 @@
       <c r="E137" s="2">
         <v>621</v>
       </c>
-      <c r="F137" s="2"/>
+      <c r="F137" s="2">
+        <v>29550</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="15">
       <c r="A138" s="2" t="s">
@@ -6354,7 +6360,9 @@
       <c r="E138" s="2">
         <v>621</v>
       </c>
-      <c r="F138" s="2"/>
+      <c r="F138" s="2">
+        <v>29550</v>
+      </c>
     </row>
     <row r="139" spans="1:6" ht="15">
       <c r="A139" s="2" t="s">
@@ -6372,7 +6380,9 @@
       <c r="E139" s="2">
         <v>621</v>
       </c>
-      <c r="F139" s="2"/>
+      <c r="F139" s="2">
+        <v>29550</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6384,8 +6394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I138" sqref="I138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8451,7 +8461,9 @@
       <c r="E103" s="4">
         <v>568</v>
       </c>
-      <c r="F103" s="4"/>
+      <c r="F103" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="15">
       <c r="A104" s="4">
@@ -8469,7 +8481,9 @@
       <c r="E104" s="4">
         <v>568</v>
       </c>
-      <c r="F104" s="4"/>
+      <c r="F104" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="15">
       <c r="A105" s="4">
@@ -8487,7 +8501,9 @@
       <c r="E105" s="4">
         <v>568</v>
       </c>
-      <c r="F105" s="4"/>
+      <c r="F105" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="15">
       <c r="A106" s="4">
@@ -8505,7 +8521,9 @@
       <c r="E106" s="4">
         <v>568</v>
       </c>
-      <c r="F106" s="4"/>
+      <c r="F106" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="15">
       <c r="A107" s="4">
@@ -8523,7 +8541,9 @@
       <c r="E107" s="4">
         <v>568</v>
       </c>
-      <c r="F107" s="4"/>
+      <c r="F107" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="15">
       <c r="A108" s="4">
@@ -8539,7 +8559,9 @@
         <v>0</v>
       </c>
       <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
+      <c r="F108" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="15">
       <c r="A109" s="4">
@@ -8557,7 +8579,9 @@
       <c r="E109" s="4">
         <v>568</v>
       </c>
-      <c r="F109" s="4"/>
+      <c r="F109" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="110" spans="1:6" ht="15">
       <c r="A110" s="4">
@@ -8575,7 +8599,9 @@
       <c r="E110" s="4">
         <v>568</v>
       </c>
-      <c r="F110" s="4"/>
+      <c r="F110" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="15">
       <c r="A111" s="4">
@@ -8591,7 +8617,9 @@
         <v>0</v>
       </c>
       <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
+      <c r="F111" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="112" spans="1:6" ht="15">
       <c r="A112" s="4">
@@ -8609,7 +8637,9 @@
       <c r="E112" s="4">
         <v>568</v>
       </c>
-      <c r="F112" s="4"/>
+      <c r="F112" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="113" spans="1:6" ht="15">
       <c r="A113" s="4">
@@ -8627,7 +8657,9 @@
       <c r="E113" s="4">
         <v>568</v>
       </c>
-      <c r="F113" s="4"/>
+      <c r="F113" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="114" spans="1:6" ht="15">
       <c r="A114" s="4">
@@ -8643,7 +8675,9 @@
         <v>0</v>
       </c>
       <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
+      <c r="F114" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="15">
       <c r="A115" s="4">
@@ -8661,7 +8695,9 @@
       <c r="E115" s="4">
         <v>568</v>
       </c>
-      <c r="F115" s="4"/>
+      <c r="F115" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="116" spans="1:6" ht="15">
       <c r="A116" s="4">
@@ -8679,7 +8715,9 @@
       <c r="E116" s="4">
         <v>568</v>
       </c>
-      <c r="F116" s="4"/>
+      <c r="F116" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="15">
       <c r="A117" s="4">
@@ -8697,7 +8735,9 @@
       <c r="E117" s="4">
         <v>568</v>
       </c>
-      <c r="F117" s="4"/>
+      <c r="F117" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="118" spans="1:6" ht="15">
       <c r="A118" s="4">
@@ -8715,7 +8755,9 @@
       <c r="E118" s="4">
         <v>568</v>
       </c>
-      <c r="F118" s="4"/>
+      <c r="F118" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="119" spans="1:6" ht="15">
       <c r="A119" s="4">
@@ -8733,7 +8775,9 @@
       <c r="E119" s="4">
         <v>568</v>
       </c>
-      <c r="F119" s="4"/>
+      <c r="F119" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="120" spans="1:6" ht="15">
       <c r="A120" s="4">
@@ -8751,7 +8795,9 @@
       <c r="E120" s="4">
         <v>568</v>
       </c>
-      <c r="F120" s="4"/>
+      <c r="F120" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="121" spans="1:6" ht="15">
       <c r="A121" s="4">
@@ -8769,7 +8815,9 @@
       <c r="E121" s="4">
         <v>568</v>
       </c>
-      <c r="F121" s="4"/>
+      <c r="F121" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="122" spans="1:6" ht="15">
       <c r="A122" s="4">
@@ -8787,7 +8835,9 @@
       <c r="E122" s="4">
         <v>568</v>
       </c>
-      <c r="F122" s="4"/>
+      <c r="F122" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="15">
       <c r="A123" s="4">
@@ -8805,7 +8855,9 @@
       <c r="E123" s="4">
         <v>568</v>
       </c>
-      <c r="F123" s="4"/>
+      <c r="F123" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="124" spans="1:6" ht="15">
       <c r="A124" s="4">
@@ -8823,7 +8875,9 @@
       <c r="E124" s="4">
         <v>568</v>
       </c>
-      <c r="F124" s="4"/>
+      <c r="F124" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="15">
       <c r="A125" s="4">
@@ -8841,7 +8895,9 @@
       <c r="E125" s="4">
         <v>568</v>
       </c>
-      <c r="F125" s="4"/>
+      <c r="F125" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="15">
       <c r="A126" s="4">
@@ -8859,7 +8915,9 @@
       <c r="E126" s="4">
         <v>568</v>
       </c>
-      <c r="F126" s="4"/>
+      <c r="F126" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="15">
       <c r="A127" s="4">
@@ -8877,7 +8935,9 @@
       <c r="E127" s="4">
         <v>568</v>
       </c>
-      <c r="F127" s="4"/>
+      <c r="F127" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="15">
       <c r="A128" s="4">
@@ -8895,7 +8955,9 @@
       <c r="E128" s="4">
         <v>568</v>
       </c>
-      <c r="F128" s="4"/>
+      <c r="F128" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="15">
       <c r="A129" s="4">
@@ -8913,7 +8975,9 @@
       <c r="E129" s="4">
         <v>568</v>
       </c>
-      <c r="F129" s="4"/>
+      <c r="F129" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="130" spans="1:6" ht="15">
       <c r="A130" s="4">
@@ -8931,7 +8995,9 @@
       <c r="E130" s="4">
         <v>568</v>
       </c>
-      <c r="F130" s="4"/>
+      <c r="F130" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="131" spans="1:6" ht="15">
       <c r="A131" s="4">
@@ -8949,7 +9015,9 @@
       <c r="E131" s="4">
         <v>568</v>
       </c>
-      <c r="F131" s="4"/>
+      <c r="F131" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="132" spans="1:6" ht="15">
       <c r="A132" s="4">
@@ -8967,7 +9035,9 @@
       <c r="E132" s="4">
         <v>568</v>
       </c>
-      <c r="F132" s="4"/>
+      <c r="F132" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="133" spans="1:6" ht="15">
       <c r="A133" s="4">
@@ -8985,7 +9055,9 @@
       <c r="E133" s="4">
         <v>568</v>
       </c>
-      <c r="F133" s="4"/>
+      <c r="F133" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="134" spans="1:6" ht="15">
       <c r="A134" s="4">
@@ -9003,7 +9075,9 @@
       <c r="E134" s="4">
         <v>568</v>
       </c>
-      <c r="F134" s="4"/>
+      <c r="F134" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="15">
       <c r="A135" s="4">
@@ -9021,7 +9095,9 @@
       <c r="E135" s="4">
         <v>568</v>
       </c>
-      <c r="F135" s="4"/>
+      <c r="F135" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="15">
       <c r="A136" s="4">
@@ -9037,7 +9113,9 @@
         <v>0</v>
       </c>
       <c r="E136" s="4"/>
-      <c r="F136" s="4"/>
+      <c r="F136" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="15">
       <c r="A137" s="4">
@@ -9055,7 +9133,9 @@
       <c r="E137" s="4">
         <v>568</v>
       </c>
-      <c r="F137" s="4"/>
+      <c r="F137" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="15">
       <c r="A138" s="4">
@@ -9073,7 +9153,9 @@
       <c r="E138" s="4">
         <v>568</v>
       </c>
-      <c r="F138" s="4"/>
+      <c r="F138" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="139" spans="1:6" ht="15">
       <c r="A139" s="4">
@@ -9091,7 +9173,9 @@
       <c r="E139" s="4">
         <v>568</v>
       </c>
-      <c r="F139" s="4"/>
+      <c r="F139" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="140" spans="1:6" ht="15">
       <c r="A140" s="4">
@@ -9109,7 +9193,9 @@
       <c r="E140" s="4">
         <v>568</v>
       </c>
-      <c r="F140" s="4"/>
+      <c r="F140" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="141" spans="1:6" ht="15">
       <c r="A141" s="4">
@@ -9127,7 +9213,9 @@
       <c r="E141" s="4">
         <v>568</v>
       </c>
-      <c r="F141" s="4"/>
+      <c r="F141" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="142" spans="1:6" ht="15">
       <c r="A142" s="4">
@@ -9145,7 +9233,9 @@
       <c r="E142" s="4">
         <v>568</v>
       </c>
-      <c r="F142" s="4"/>
+      <c r="F142" s="4">
+        <v>30392</v>
+      </c>
     </row>
     <row r="143" spans="1:6" ht="15">
       <c r="A143" s="4">
@@ -9163,7 +9253,9 @@
       <c r="E143" s="4">
         <v>568</v>
       </c>
-      <c r="F143" s="4"/>
+      <c r="F143" s="4">
+        <v>30392</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -9175,8 +9267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E161" sqref="E161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11340,7 +11432,9 @@
       <c r="E108" s="5">
         <v>585</v>
       </c>
-      <c r="F108" s="5"/>
+      <c r="F108" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="30">
       <c r="A109" s="5">
@@ -11358,7 +11452,9 @@
       <c r="E109" s="5">
         <v>585</v>
       </c>
-      <c r="F109" s="5"/>
+      <c r="F109" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="110" spans="1:6" ht="30">
       <c r="A110" s="5">
@@ -11376,7 +11472,9 @@
       <c r="E110" s="5">
         <v>585</v>
       </c>
-      <c r="F110" s="5"/>
+      <c r="F110" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="30">
       <c r="A111" s="5">
@@ -11392,7 +11490,9 @@
         <v>0</v>
       </c>
       <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
+      <c r="F111" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="112" spans="1:6" ht="45">
       <c r="A112" s="5">
@@ -11408,7 +11508,9 @@
         <v>0</v>
       </c>
       <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
+      <c r="F112" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="113" spans="1:6" ht="30">
       <c r="A113" s="5">
@@ -11426,7 +11528,9 @@
       <c r="E113" s="5">
         <v>585</v>
       </c>
-      <c r="F113" s="5"/>
+      <c r="F113" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="114" spans="1:6" ht="30">
       <c r="A114" s="5">
@@ -11442,7 +11546,9 @@
         <v>0</v>
       </c>
       <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
+      <c r="F114" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="30">
       <c r="A115" s="5">
@@ -11460,7 +11566,9 @@
       <c r="E115" s="5">
         <v>585</v>
       </c>
-      <c r="F115" s="5"/>
+      <c r="F115" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="116" spans="1:6" ht="45">
       <c r="A116" s="5">
@@ -11478,7 +11586,9 @@
       <c r="E116" s="5">
         <v>585</v>
       </c>
-      <c r="F116" s="5"/>
+      <c r="F116" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="30">
       <c r="A117" s="5">
@@ -11494,7 +11604,9 @@
         <v>0</v>
       </c>
       <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
+      <c r="F117" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="118" spans="1:6" ht="30">
       <c r="A118" s="5">
@@ -11510,7 +11622,9 @@
         <v>0</v>
       </c>
       <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
+      <c r="F118" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="119" spans="1:6" ht="45">
       <c r="A119" s="5">
@@ -11528,7 +11642,9 @@
       <c r="E119" s="5">
         <v>585</v>
       </c>
-      <c r="F119" s="5"/>
+      <c r="F119" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="120" spans="1:6" ht="30">
       <c r="A120" s="5">
@@ -11546,7 +11662,9 @@
       <c r="E120" s="5">
         <v>585</v>
       </c>
-      <c r="F120" s="5"/>
+      <c r="F120" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="121" spans="1:6" ht="30">
       <c r="A121" s="5">
@@ -11564,7 +11682,9 @@
       <c r="E121" s="5">
         <v>585</v>
       </c>
-      <c r="F121" s="5"/>
+      <c r="F121" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="122" spans="1:6" ht="30">
       <c r="A122" s="5">
@@ -11582,7 +11702,9 @@
       <c r="E122" s="5">
         <v>585</v>
       </c>
-      <c r="F122" s="5"/>
+      <c r="F122" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="30">
       <c r="A123" s="5">
@@ -11600,7 +11722,9 @@
       <c r="E123" s="5">
         <v>585</v>
       </c>
-      <c r="F123" s="5"/>
+      <c r="F123" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="124" spans="1:6" ht="30">
       <c r="A124" s="5">
@@ -11618,7 +11742,9 @@
       <c r="E124" s="5">
         <v>585</v>
       </c>
-      <c r="F124" s="5"/>
+      <c r="F124" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="30">
       <c r="A125" s="5">
@@ -11636,7 +11762,9 @@
       <c r="E125" s="5">
         <v>585</v>
       </c>
-      <c r="F125" s="5"/>
+      <c r="F125" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="30">
       <c r="A126" s="5">
@@ -11654,7 +11782,9 @@
       <c r="E126" s="5">
         <v>585</v>
       </c>
-      <c r="F126" s="5"/>
+      <c r="F126" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="30">
       <c r="A127" s="5">
@@ -11672,7 +11802,9 @@
       <c r="E127" s="5">
         <v>585</v>
       </c>
-      <c r="F127" s="5"/>
+      <c r="F127" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="30">
       <c r="A128" s="5">
@@ -11690,7 +11822,9 @@
       <c r="E128" s="5">
         <v>585</v>
       </c>
-      <c r="F128" s="5"/>
+      <c r="F128" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="45">
       <c r="A129" s="5">
@@ -11708,7 +11842,9 @@
       <c r="E129" s="5">
         <v>585</v>
       </c>
-      <c r="F129" s="5"/>
+      <c r="F129" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="130" spans="1:6" ht="30">
       <c r="A130" s="5">
@@ -11726,7 +11862,9 @@
       <c r="E130" s="5">
         <v>585</v>
       </c>
-      <c r="F130" s="5"/>
+      <c r="F130" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="131" spans="1:6" ht="30">
       <c r="A131" s="5">
@@ -11744,7 +11882,9 @@
       <c r="E131" s="5">
         <v>585</v>
       </c>
-      <c r="F131" s="5"/>
+      <c r="F131" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="132" spans="1:6" ht="45">
       <c r="A132" s="5">
@@ -11762,7 +11902,9 @@
       <c r="E132" s="5">
         <v>585</v>
       </c>
-      <c r="F132" s="5"/>
+      <c r="F132" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="133" spans="1:6" ht="30">
       <c r="A133" s="5">
@@ -11780,7 +11922,9 @@
       <c r="E133" s="5">
         <v>585</v>
       </c>
-      <c r="F133" s="5"/>
+      <c r="F133" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="134" spans="1:6" ht="30">
       <c r="A134" s="5">
@@ -11798,7 +11942,9 @@
       <c r="E134" s="5">
         <v>585</v>
       </c>
-      <c r="F134" s="5"/>
+      <c r="F134" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="30">
       <c r="A135" s="5">
@@ -11816,7 +11962,9 @@
       <c r="E135" s="5">
         <v>585</v>
       </c>
-      <c r="F135" s="5"/>
+      <c r="F135" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="30">
       <c r="A136" s="5">
@@ -11834,7 +11982,9 @@
       <c r="E136" s="5">
         <v>585</v>
       </c>
-      <c r="F136" s="5"/>
+      <c r="F136" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="30">
       <c r="A137" s="5">
@@ -11852,7 +12002,9 @@
       <c r="E137" s="5">
         <v>585</v>
       </c>
-      <c r="F137" s="5"/>
+      <c r="F137" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="30">
       <c r="A138" s="5">
@@ -11870,7 +12022,9 @@
       <c r="E138" s="5">
         <v>585</v>
       </c>
-      <c r="F138" s="5"/>
+      <c r="F138" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="139" spans="1:6" ht="30">
       <c r="A139" s="5">
@@ -11886,7 +12040,9 @@
         <v>0</v>
       </c>
       <c r="E139" s="5"/>
-      <c r="F139" s="5"/>
+      <c r="F139" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="140" spans="1:6" ht="45">
       <c r="A140" s="5">
@@ -11904,7 +12060,9 @@
       <c r="E140" s="5">
         <v>585</v>
       </c>
-      <c r="F140" s="5"/>
+      <c r="F140" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="141" spans="1:6" ht="30">
       <c r="A141" s="5">
@@ -11922,7 +12080,9 @@
       <c r="E141" s="5">
         <v>585</v>
       </c>
-      <c r="F141" s="5"/>
+      <c r="F141" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="142" spans="1:6" ht="30">
       <c r="A142" s="5">
@@ -11938,7 +12098,9 @@
         <v>0</v>
       </c>
       <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
+      <c r="F142" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="143" spans="1:6" ht="45">
       <c r="A143" s="5">
@@ -11956,7 +12118,9 @@
       <c r="E143" s="5">
         <v>585</v>
       </c>
-      <c r="F143" s="5"/>
+      <c r="F143" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="144" spans="1:6" ht="30">
       <c r="A144" s="5">
@@ -11974,7 +12138,9 @@
       <c r="E144" s="5">
         <v>585</v>
       </c>
-      <c r="F144" s="5"/>
+      <c r="F144" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="145" spans="1:6" ht="45">
       <c r="A145" s="5">
@@ -11992,7 +12158,9 @@
       <c r="E145" s="5">
         <v>585</v>
       </c>
-      <c r="F145" s="5"/>
+      <c r="F145" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="146" spans="1:6" ht="60">
       <c r="A146" s="5">
@@ -12010,752 +12178,336 @@
       <c r="E146" s="5">
         <v>585</v>
       </c>
-      <c r="F146" s="5"/>
+      <c r="F146" s="5">
+        <v>29207</v>
+      </c>
     </row>
     <row r="147" spans="1:6" ht="16.5">
-      <c r="A147" s="7">
-        <v>10140</v>
-      </c>
-      <c r="B147" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C147" s="7">
-        <v>14</v>
-      </c>
-      <c r="D147" s="7">
-        <v>14</v>
-      </c>
-      <c r="E147" s="7">
-        <v>578</v>
-      </c>
-      <c r="F147" s="7">
-        <v>49276</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="28.5">
-      <c r="A148" s="7">
-        <v>10254</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="C148" s="7">
-        <v>127</v>
-      </c>
-      <c r="D148" s="7">
-        <v>127</v>
-      </c>
-      <c r="E148" s="7">
-        <v>577</v>
-      </c>
-      <c r="F148" s="7">
-        <v>50373</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="28.5">
-      <c r="A149" s="7">
-        <v>10700</v>
-      </c>
-      <c r="B149" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="C149" s="7">
-        <v>36</v>
-      </c>
-      <c r="D149" s="7">
-        <v>43</v>
-      </c>
-      <c r="E149" s="7">
-        <v>577</v>
-      </c>
-      <c r="F149" s="7">
-        <v>50470</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="42.75">
-      <c r="A150" s="7">
-        <v>19145</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C150" s="7">
-        <v>67</v>
-      </c>
-      <c r="D150" s="7">
-        <v>67</v>
-      </c>
-      <c r="E150" s="7">
-        <v>577</v>
-      </c>
-      <c r="F150" s="7">
-        <v>50561</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="28.5">
-      <c r="A151" s="7">
-        <v>10226</v>
-      </c>
-      <c r="B151" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C151" s="7">
-        <v>27</v>
-      </c>
-      <c r="D151" s="7">
-        <v>28</v>
-      </c>
-      <c r="E151" s="7">
-        <v>577</v>
-      </c>
-      <c r="F151" s="7">
-        <v>50691</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="28.5">
-      <c r="A152" s="7">
-        <v>10490</v>
-      </c>
-      <c r="B152" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="C152" s="7">
-        <v>34</v>
-      </c>
-      <c r="D152" s="7">
-        <v>34</v>
-      </c>
-      <c r="E152" s="7">
-        <v>577</v>
-      </c>
-      <c r="F152" s="7">
-        <v>50820</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="28.5">
-      <c r="A153" s="7">
-        <v>10107</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C153" s="7">
-        <v>13</v>
-      </c>
-      <c r="D153" s="7">
-        <v>1</v>
-      </c>
-      <c r="E153" s="7">
-        <v>577</v>
-      </c>
+      <c r="A147" s="7"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="5"/>
+    </row>
+    <row r="148" spans="1:6" ht="16.5">
+      <c r="A148" s="7"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
+    </row>
+    <row r="149" spans="1:6" ht="16.5">
+      <c r="A149" s="7"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+    </row>
+    <row r="150" spans="1:6" ht="16.5">
+      <c r="A150" s="7"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+    </row>
+    <row r="151" spans="1:6" ht="16.5">
+      <c r="A151" s="7"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="7"/>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
+    </row>
+    <row r="152" spans="1:6" ht="16.5">
+      <c r="A152" s="7"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
+    </row>
+    <row r="153" spans="1:6" ht="16.5">
+      <c r="A153" s="7"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="7"/>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
       <c r="F153" s="7"/>
     </row>
     <row r="154" spans="1:6" ht="16.5">
-      <c r="A154" s="7">
-        <v>10110</v>
-      </c>
-      <c r="B154" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C154" s="7">
-        <v>94</v>
-      </c>
-      <c r="D154" s="7">
-        <v>4</v>
-      </c>
-      <c r="E154" s="7">
-        <v>577</v>
-      </c>
+      <c r="A154" s="7"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="7"/>
+      <c r="D154" s="7"/>
+      <c r="E154" s="7"/>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="1:6" ht="28.5">
-      <c r="A155" s="7">
-        <v>10126</v>
-      </c>
-      <c r="B155" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C155" s="7">
-        <v>41</v>
-      </c>
-      <c r="D155" s="7">
-        <v>3</v>
-      </c>
-      <c r="E155" s="7">
-        <v>577</v>
-      </c>
+    <row r="155" spans="1:6" ht="16.5">
+      <c r="A155" s="7"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="1:6" ht="28.5">
-      <c r="A156" s="7">
-        <v>10147</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C156" s="7">
-        <v>18</v>
-      </c>
-      <c r="D156" s="7">
-        <v>1</v>
-      </c>
-      <c r="E156" s="7">
-        <v>577</v>
-      </c>
+    <row r="156" spans="1:6" ht="16.5">
+      <c r="A156" s="7"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="7"/>
+      <c r="D156" s="7"/>
+      <c r="E156" s="7"/>
       <c r="F156" s="7"/>
     </row>
     <row r="157" spans="1:6" ht="16.5">
-      <c r="A157" s="7">
-        <v>10184</v>
-      </c>
-      <c r="B157" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C157" s="7">
-        <v>8</v>
-      </c>
-      <c r="D157" s="7">
-        <v>3</v>
-      </c>
-      <c r="E157" s="7">
-        <v>577</v>
-      </c>
+      <c r="A157" s="7"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="7"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7"/>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="1:6" ht="28.5">
-      <c r="A158" s="7">
-        <v>10186</v>
-      </c>
-      <c r="B158" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="C158" s="7">
-        <v>150</v>
-      </c>
-      <c r="D158" s="7">
-        <v>4</v>
-      </c>
-      <c r="E158" s="7">
-        <v>577</v>
-      </c>
+    <row r="158" spans="1:6" ht="16.5">
+      <c r="A158" s="7"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="7"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="1:6" ht="28.5">
-      <c r="A159" s="7">
-        <v>10212</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="C159" s="7">
-        <v>61</v>
-      </c>
-      <c r="D159" s="7">
-        <v>0</v>
-      </c>
+    <row r="159" spans="1:6" ht="16.5">
+      <c r="A159" s="7"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="1:6" ht="28.5">
-      <c r="A160" s="7">
-        <v>10214</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="C160" s="7">
-        <v>121</v>
-      </c>
-      <c r="D160" s="7">
-        <v>7</v>
-      </c>
-      <c r="E160" s="7">
-        <v>577</v>
-      </c>
+    <row r="160" spans="1:6" ht="16.5">
+      <c r="A160" s="7"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
       <c r="F160" s="7"/>
     </row>
     <row r="161" spans="1:6" ht="16.5">
-      <c r="A161" s="7">
-        <v>10216</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C161" s="7">
-        <v>54</v>
-      </c>
-      <c r="D161" s="7">
-        <v>51</v>
-      </c>
-      <c r="E161" s="7">
-        <v>577</v>
-      </c>
+      <c r="A161" s="7"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="1:6" ht="28.5">
-      <c r="A162" s="7">
-        <v>10220</v>
-      </c>
-      <c r="B162" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C162" s="7">
-        <v>46</v>
-      </c>
-      <c r="D162" s="7">
-        <v>0</v>
-      </c>
+    <row r="162" spans="1:6" ht="16.5">
+      <c r="A162" s="7"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="7"/>
+      <c r="D162" s="7"/>
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="1:6" ht="28.5">
-      <c r="A163" s="7">
-        <v>10224</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="C163" s="7">
-        <v>24</v>
-      </c>
-      <c r="D163" s="7">
-        <v>4</v>
-      </c>
-      <c r="E163" s="7">
-        <v>577</v>
-      </c>
+    <row r="163" spans="1:6" ht="16.5">
+      <c r="A163" s="7"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="1:6" ht="28.5">
-      <c r="A164" s="7">
-        <v>10225</v>
-      </c>
-      <c r="B164" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C164" s="7">
-        <v>24</v>
-      </c>
-      <c r="D164" s="7">
-        <v>3</v>
-      </c>
-      <c r="E164" s="7">
-        <v>577</v>
-      </c>
+    <row r="164" spans="1:6" ht="16.5">
+      <c r="A164" s="7"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="7"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="1:6" ht="28.5">
-      <c r="A165" s="7">
-        <v>10264</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="C165" s="7">
-        <v>81</v>
-      </c>
-      <c r="D165" s="7">
-        <v>59</v>
-      </c>
-      <c r="E165" s="7">
-        <v>577</v>
-      </c>
+    <row r="165" spans="1:6" ht="16.5">
+      <c r="A165" s="7"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="7"/>
+      <c r="D165" s="7"/>
+      <c r="E165" s="7"/>
       <c r="F165" s="7"/>
     </row>
-    <row r="166" spans="1:6" ht="28.5">
-      <c r="A166" s="7">
-        <v>10298</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="C166" s="7">
-        <v>80</v>
-      </c>
-      <c r="D166" s="7">
-        <v>13</v>
-      </c>
-      <c r="E166" s="7">
-        <v>577</v>
-      </c>
+    <row r="166" spans="1:6" ht="16.5">
+      <c r="A166" s="7"/>
+      <c r="B166" s="8"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
       <c r="F166" s="7"/>
     </row>
-    <row r="167" spans="1:6" ht="28.5">
-      <c r="A167" s="7">
-        <v>10366</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C167" s="7">
-        <v>8</v>
-      </c>
-      <c r="D167" s="7">
-        <v>7</v>
-      </c>
-      <c r="E167" s="7">
-        <v>577</v>
-      </c>
+    <row r="167" spans="1:6" ht="16.5">
+      <c r="A167" s="7"/>
+      <c r="B167" s="8"/>
+      <c r="C167" s="7"/>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7"/>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="1:6" ht="28.5">
-      <c r="A168" s="7">
-        <v>10394</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="C168" s="7">
-        <v>52</v>
-      </c>
-      <c r="D168" s="7">
-        <v>12</v>
-      </c>
-      <c r="E168" s="7">
-        <v>577</v>
-      </c>
+    <row r="168" spans="1:6" ht="16.5">
+      <c r="A168" s="7"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="7"/>
+      <c r="D168" s="7"/>
+      <c r="E168" s="7"/>
       <c r="F168" s="7"/>
     </row>
-    <row r="169" spans="1:6" ht="28.5">
-      <c r="A169" s="7">
-        <v>10404</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="C169" s="7">
-        <v>59</v>
-      </c>
-      <c r="D169" s="7">
-        <v>17</v>
-      </c>
-      <c r="E169" s="7">
-        <v>577</v>
-      </c>
+    <row r="169" spans="1:6" ht="16.5">
+      <c r="A169" s="7"/>
+      <c r="B169" s="8"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="7"/>
+      <c r="E169" s="7"/>
       <c r="F169" s="7"/>
     </row>
-    <row r="170" spans="1:6" ht="28.5">
-      <c r="A170" s="7">
-        <v>10407</v>
-      </c>
-      <c r="B170" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C170" s="7">
-        <v>100</v>
-      </c>
-      <c r="D170" s="7">
-        <v>2</v>
-      </c>
-      <c r="E170" s="7">
-        <v>577</v>
-      </c>
+    <row r="170" spans="1:6" ht="16.5">
+      <c r="A170" s="7"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="7"/>
+      <c r="D170" s="7"/>
+      <c r="E170" s="7"/>
       <c r="F170" s="7"/>
     </row>
     <row r="171" spans="1:6" ht="16.5">
-      <c r="A171" s="7">
-        <v>10427</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C171" s="7">
-        <v>100</v>
-      </c>
-      <c r="D171" s="7">
-        <v>5</v>
-      </c>
-      <c r="E171" s="7">
-        <v>577</v>
-      </c>
+      <c r="A171" s="7"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="7"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="7"/>
       <c r="F171" s="7"/>
     </row>
     <row r="172" spans="1:6" ht="16.5">
-      <c r="A172" s="7">
-        <v>10475</v>
-      </c>
-      <c r="B172" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="C172" s="7">
-        <v>94</v>
-      </c>
-      <c r="D172" s="7">
-        <v>1</v>
-      </c>
-      <c r="E172" s="7">
-        <v>577</v>
-      </c>
+      <c r="A172" s="7"/>
+      <c r="B172" s="8"/>
+      <c r="C172" s="7"/>
+      <c r="D172" s="7"/>
+      <c r="E172" s="7"/>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="1:6" ht="28.5">
-      <c r="A173" s="7">
-        <v>10534</v>
-      </c>
-      <c r="B173" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C173" s="7">
-        <v>72</v>
-      </c>
-      <c r="D173" s="7">
-        <v>7</v>
-      </c>
-      <c r="E173" s="7">
-        <v>577</v>
-      </c>
+    <row r="173" spans="1:6" ht="16.5">
+      <c r="A173" s="7"/>
+      <c r="B173" s="8"/>
+      <c r="C173" s="7"/>
+      <c r="D173" s="7"/>
+      <c r="E173" s="7"/>
       <c r="F173" s="7"/>
     </row>
-    <row r="174" spans="1:6" ht="28.5">
-      <c r="A174" s="7">
-        <v>10536</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="C174" s="7">
-        <v>161</v>
-      </c>
-      <c r="D174" s="7">
-        <v>83</v>
-      </c>
-      <c r="E174" s="7">
-        <v>577</v>
-      </c>
+    <row r="174" spans="1:6" ht="16.5">
+      <c r="A174" s="7"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="7"/>
+      <c r="D174" s="7"/>
+      <c r="E174" s="7"/>
       <c r="F174" s="7"/>
     </row>
-    <row r="175" spans="1:6" ht="28.5">
-      <c r="A175" s="7">
-        <v>10537</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="C175" s="7">
-        <v>130</v>
-      </c>
-      <c r="D175" s="7">
-        <v>4</v>
-      </c>
-      <c r="E175" s="7">
-        <v>577</v>
-      </c>
+    <row r="175" spans="1:6" ht="16.5">
+      <c r="A175" s="7"/>
+      <c r="B175" s="8"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7"/>
       <c r="F175" s="7"/>
     </row>
-    <row r="176" spans="1:6" ht="28.5">
-      <c r="A176" s="7">
-        <v>10538</v>
-      </c>
-      <c r="B176" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C176" s="7">
-        <v>94</v>
-      </c>
-      <c r="D176" s="7">
-        <v>1</v>
-      </c>
-      <c r="E176" s="7">
-        <v>577</v>
-      </c>
+    <row r="176" spans="1:6" ht="16.5">
+      <c r="A176" s="7"/>
+      <c r="B176" s="8"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
       <c r="F176" s="7"/>
     </row>
     <row r="177" spans="1:6" ht="16.5">
-      <c r="A177" s="7">
-        <v>10555</v>
-      </c>
-      <c r="B177" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="C177" s="7">
-        <v>180</v>
-      </c>
-      <c r="D177" s="7">
-        <v>28</v>
-      </c>
-      <c r="E177" s="7">
-        <v>577</v>
-      </c>
+      <c r="A177" s="7"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="7"/>
+      <c r="E177" s="7"/>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="1:6" ht="28.5">
-      <c r="A178" s="7">
-        <v>10566</v>
-      </c>
-      <c r="B178" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="C178" s="7">
-        <v>1311</v>
-      </c>
-      <c r="D178" s="7">
-        <v>150</v>
-      </c>
-      <c r="E178" s="7">
-        <v>577</v>
-      </c>
+    <row r="178" spans="1:6" ht="16.5">
+      <c r="A178" s="7"/>
+      <c r="B178" s="8"/>
+      <c r="C178" s="7"/>
+      <c r="D178" s="7"/>
+      <c r="E178" s="7"/>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="1:6" ht="28.5">
-      <c r="A179" s="7">
-        <v>10571</v>
-      </c>
-      <c r="B179" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="C179" s="7">
-        <v>688</v>
-      </c>
-      <c r="D179" s="7">
-        <v>601</v>
-      </c>
-      <c r="E179" s="7">
-        <v>577</v>
-      </c>
+    <row r="179" spans="1:6" ht="16.5">
+      <c r="A179" s="7"/>
+      <c r="B179" s="8"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="7"/>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="1:6" ht="28.5">
-      <c r="A180" s="7">
-        <v>10572</v>
-      </c>
-      <c r="B180" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="C180" s="7">
-        <v>1299</v>
-      </c>
-      <c r="D180" s="7">
-        <v>1284</v>
-      </c>
-      <c r="E180" s="7">
-        <v>577</v>
-      </c>
+    <row r="180" spans="1:6" ht="16.5">
+      <c r="A180" s="7"/>
+      <c r="B180" s="8"/>
+      <c r="C180" s="7"/>
+      <c r="D180" s="7"/>
+      <c r="E180" s="7"/>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="1:6" ht="28.5">
-      <c r="A181" s="7">
-        <v>10616</v>
-      </c>
-      <c r="B181" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C181" s="7">
-        <v>64</v>
-      </c>
-      <c r="D181" s="7">
-        <v>12</v>
-      </c>
-      <c r="E181" s="7">
-        <v>577</v>
-      </c>
+    <row r="181" spans="1:6" ht="16.5">
+      <c r="A181" s="7"/>
+      <c r="B181" s="8"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7"/>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="1:6" ht="28.5">
-      <c r="A182" s="7">
-        <v>10626</v>
-      </c>
-      <c r="B182" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="C182" s="7">
-        <v>10</v>
-      </c>
-      <c r="D182" s="7">
-        <v>5</v>
-      </c>
-      <c r="E182" s="7">
-        <v>577</v>
-      </c>
+    <row r="182" spans="1:6" ht="16.5">
+      <c r="A182" s="7"/>
+      <c r="B182" s="8"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="1:6" ht="28.5">
-      <c r="A183" s="7">
-        <v>10708</v>
-      </c>
-      <c r="B183" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C183" s="7">
-        <v>15</v>
-      </c>
-      <c r="D183" s="7">
-        <v>2</v>
-      </c>
-      <c r="E183" s="7">
-        <v>577</v>
-      </c>
+    <row r="183" spans="1:6" ht="16.5">
+      <c r="A183" s="7"/>
+      <c r="B183" s="8"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="1:6" ht="47.25">
-      <c r="A184" s="7">
-        <v>11414</v>
-      </c>
-      <c r="B184" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="C184" s="7">
-        <v>19</v>
-      </c>
-      <c r="D184" s="7">
-        <v>16</v>
-      </c>
-      <c r="E184" s="7">
-        <v>577</v>
-      </c>
+    <row r="184" spans="1:6" ht="16.5">
+      <c r="A184" s="7"/>
+      <c r="B184" s="8"/>
+      <c r="C184" s="7"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7"/>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="1:6" ht="47.25">
-      <c r="A185" s="7">
-        <v>19635</v>
-      </c>
-      <c r="B185" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C185" s="7">
-        <v>48</v>
-      </c>
-      <c r="D185" s="7">
-        <v>1</v>
-      </c>
-      <c r="E185" s="7">
-        <v>577</v>
-      </c>
+    <row r="185" spans="1:6" ht="16.5">
+      <c r="A185" s="7"/>
+      <c r="B185" s="8"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7"/>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="1:6" ht="61.5">
-      <c r="A186" s="7">
-        <v>60145</v>
-      </c>
-      <c r="B186" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C186" s="7">
-        <v>15</v>
-      </c>
-      <c r="D186" s="7">
-        <v>11</v>
-      </c>
-      <c r="E186" s="7">
-        <v>577</v>
-      </c>
+    <row r="186" spans="1:6" ht="16.5">
+      <c r="A186" s="7"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="7"/>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="1:6" ht="61.5">
-      <c r="A187" s="7">
-        <v>60173</v>
-      </c>
-      <c r="B187" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C187" s="7">
-        <v>10</v>
-      </c>
-      <c r="D187" s="7">
-        <v>2</v>
-      </c>
-      <c r="E187" s="7">
-        <v>577</v>
-      </c>
+    <row r="187" spans="1:6" ht="16.5">
+      <c r="A187" s="7"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
       <c r="F187" s="7"/>
     </row>
   </sheetData>
@@ -12766,10 +12518,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15073,7 +14825,9 @@
       <c r="E115" s="12">
         <v>574</v>
       </c>
-      <c r="F115" s="13"/>
+      <c r="F115" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="116" spans="1:6" ht="45">
       <c r="A116" s="11">
@@ -15091,7 +14845,9 @@
       <c r="E116" s="12">
         <v>574</v>
       </c>
-      <c r="F116" s="13"/>
+      <c r="F116" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="117" spans="1:6" ht="30">
       <c r="A117" s="11">
@@ -15109,7 +14865,9 @@
       <c r="E117" s="12">
         <v>574</v>
       </c>
-      <c r="F117" s="13"/>
+      <c r="F117" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="118" spans="1:6" ht="45">
       <c r="A118" s="11">
@@ -15127,7 +14885,9 @@
       <c r="E118" s="12">
         <v>574</v>
       </c>
-      <c r="F118" s="13"/>
+      <c r="F118" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="119" spans="1:6" ht="30">
       <c r="A119" s="11">
@@ -15145,7 +14905,9 @@
       <c r="E119" s="12">
         <v>574</v>
       </c>
-      <c r="F119" s="13"/>
+      <c r="F119" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="120" spans="1:6" ht="30">
       <c r="A120" s="11">
@@ -15161,7 +14923,9 @@
         <v>0</v>
       </c>
       <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
+      <c r="F120" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="121" spans="1:6" ht="30">
       <c r="A121" s="11">
@@ -15179,7 +14943,9 @@
       <c r="E121" s="12">
         <v>574</v>
       </c>
-      <c r="F121" s="13"/>
+      <c r="F121" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="122" spans="1:6" ht="45">
       <c r="A122" s="11">
@@ -15195,7 +14961,9 @@
         <v>0</v>
       </c>
       <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
+      <c r="F122" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="30">
       <c r="A123" s="11">
@@ -15213,7 +14981,9 @@
       <c r="E123" s="12">
         <v>574</v>
       </c>
-      <c r="F123" s="13"/>
+      <c r="F123" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="124" spans="1:6" ht="30">
       <c r="A124" s="11">
@@ -15231,7 +15001,9 @@
       <c r="E124" s="12">
         <v>574</v>
       </c>
-      <c r="F124" s="13"/>
+      <c r="F124" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="30">
       <c r="A125" s="11">
@@ -15249,7 +15021,9 @@
       <c r="E125" s="12">
         <v>574</v>
       </c>
-      <c r="F125" s="13"/>
+      <c r="F125" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="30">
       <c r="A126" s="11">
@@ -15267,7 +15041,9 @@
       <c r="E126" s="12">
         <v>574</v>
       </c>
-      <c r="F126" s="13"/>
+      <c r="F126" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="30">
       <c r="A127" s="11">
@@ -15285,7 +15061,9 @@
       <c r="E127" s="12">
         <v>574</v>
       </c>
-      <c r="F127" s="13"/>
+      <c r="F127" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="30">
       <c r="A128" s="11">
@@ -15301,7 +15079,9 @@
         <v>0</v>
       </c>
       <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
+      <c r="F128" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="30">
       <c r="A129" s="11">
@@ -15319,7 +15099,9 @@
       <c r="E129" s="12">
         <v>574</v>
       </c>
-      <c r="F129" s="13"/>
+      <c r="F129" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="130" spans="1:6" ht="30">
       <c r="A130" s="11">
@@ -15337,7 +15119,9 @@
       <c r="E130" s="12">
         <v>574</v>
       </c>
-      <c r="F130" s="13"/>
+      <c r="F130" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="131" spans="1:6" ht="30">
       <c r="A131" s="11">
@@ -15355,7 +15139,9 @@
       <c r="E131" s="12">
         <v>574</v>
       </c>
-      <c r="F131" s="13"/>
+      <c r="F131" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="132" spans="1:6" ht="30">
       <c r="A132" s="11">
@@ -15373,7 +15159,9 @@
       <c r="E132" s="12">
         <v>574</v>
       </c>
-      <c r="F132" s="13"/>
+      <c r="F132" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="133" spans="1:6" ht="30">
       <c r="A133" s="11">
@@ -15391,7 +15179,9 @@
       <c r="E133" s="12">
         <v>574</v>
       </c>
-      <c r="F133" s="13"/>
+      <c r="F133" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="134" spans="1:6" ht="45">
       <c r="A134" s="11">
@@ -15409,7 +15199,9 @@
       <c r="E134" s="12">
         <v>574</v>
       </c>
-      <c r="F134" s="13"/>
+      <c r="F134" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="45">
       <c r="A135" s="11">
@@ -15427,7 +15219,9 @@
       <c r="E135" s="12">
         <v>574</v>
       </c>
-      <c r="F135" s="13"/>
+      <c r="F135" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="30">
       <c r="A136" s="11">
@@ -15445,7 +15239,9 @@
       <c r="E136" s="12">
         <v>574</v>
       </c>
-      <c r="F136" s="13"/>
+      <c r="F136" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="30">
       <c r="A137" s="11">
@@ -15463,7 +15259,9 @@
       <c r="E137" s="12">
         <v>574</v>
       </c>
-      <c r="F137" s="13"/>
+      <c r="F137" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="30">
       <c r="A138" s="11">
@@ -15481,7 +15279,9 @@
       <c r="E138" s="12">
         <v>574</v>
       </c>
-      <c r="F138" s="13"/>
+      <c r="F138" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="139" spans="1:6" ht="45">
       <c r="A139" s="11">
@@ -15499,7 +15299,9 @@
       <c r="E139" s="12">
         <v>574</v>
       </c>
-      <c r="F139" s="13"/>
+      <c r="F139" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="140" spans="1:6" ht="30">
       <c r="A140" s="11">
@@ -15517,7 +15319,9 @@
       <c r="E140" s="12">
         <v>574</v>
       </c>
-      <c r="F140" s="13"/>
+      <c r="F140" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="141" spans="1:6" ht="30">
       <c r="A141" s="11">
@@ -15535,7 +15339,9 @@
       <c r="E141" s="12">
         <v>574</v>
       </c>
-      <c r="F141" s="13"/>
+      <c r="F141" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="142" spans="1:6" ht="30">
       <c r="A142" s="11">
@@ -15551,7 +15357,9 @@
         <v>0</v>
       </c>
       <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
+      <c r="F142" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="143" spans="1:6" ht="30">
       <c r="A143" s="11">
@@ -15569,7 +15377,9 @@
       <c r="E143" s="12">
         <v>574</v>
       </c>
-      <c r="F143" s="13"/>
+      <c r="F143" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="144" spans="1:6" ht="30">
       <c r="A144" s="11">
@@ -15587,7 +15397,9 @@
       <c r="E144" s="12">
         <v>574</v>
       </c>
-      <c r="F144" s="13"/>
+      <c r="F144" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="145" spans="1:6" ht="30">
       <c r="A145" s="11">
@@ -15603,7 +15415,9 @@
         <v>0</v>
       </c>
       <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
+      <c r="F145" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="146" spans="1:6" ht="45">
       <c r="A146" s="11">
@@ -15621,7 +15435,9 @@
       <c r="E146" s="12">
         <v>574</v>
       </c>
-      <c r="F146" s="13"/>
+      <c r="F146" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="147" spans="1:6" ht="30">
       <c r="A147" s="11">
@@ -15639,7 +15455,9 @@
       <c r="E147" s="12">
         <v>574</v>
       </c>
-      <c r="F147" s="13"/>
+      <c r="F147" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="148" spans="1:6" ht="30">
       <c r="A148" s="11">
@@ -15655,7 +15473,9 @@
         <v>0</v>
       </c>
       <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
+      <c r="F148" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="149" spans="1:6" ht="30">
       <c r="A149" s="11">
@@ -15673,7 +15493,9 @@
       <c r="E149" s="12">
         <v>574</v>
       </c>
-      <c r="F149" s="13"/>
+      <c r="F149" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="150" spans="1:6" ht="30">
       <c r="A150" s="11">
@@ -15691,7 +15513,9 @@
       <c r="E150" s="12">
         <v>574</v>
       </c>
-      <c r="F150" s="13"/>
+      <c r="F150" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="151" spans="1:6" ht="60">
       <c r="A151" s="11">
@@ -15709,7 +15533,9 @@
       <c r="E151" s="12">
         <v>574</v>
       </c>
-      <c r="F151" s="13"/>
+      <c r="F151" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="152" spans="1:6" ht="45">
       <c r="A152" s="11">
@@ -15727,7 +15553,9 @@
       <c r="E152" s="12">
         <v>574</v>
       </c>
-      <c r="F152" s="13"/>
+      <c r="F152" s="13">
+        <v>40420</v>
+      </c>
     </row>
     <row r="153" spans="1:6" ht="60">
       <c r="A153" s="11">
@@ -15745,7 +15573,12 @@
       <c r="E153" s="12">
         <v>574</v>
       </c>
-      <c r="F153" s="13"/>
+      <c r="F153" s="13">
+        <v>40420</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="F154" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -15757,8 +15590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F163" sqref="F163:F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18242,7 +18075,9 @@
       <c r="E124" s="15">
         <v>560</v>
       </c>
-      <c r="F124" s="15"/>
+      <c r="F124" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="15">
       <c r="A125" s="15">
@@ -18260,7 +18095,9 @@
       <c r="E125" s="15">
         <v>560</v>
       </c>
-      <c r="F125" s="15"/>
+      <c r="F125" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="15">
       <c r="A126" s="15">
@@ -18278,7 +18115,9 @@
       <c r="E126" s="15">
         <v>560</v>
       </c>
-      <c r="F126" s="15"/>
+      <c r="F126" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="15">
       <c r="A127" s="15">
@@ -18296,7 +18135,9 @@
       <c r="E127" s="15">
         <v>560</v>
       </c>
-      <c r="F127" s="15"/>
+      <c r="F127" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="15">
       <c r="A128" s="15">
@@ -18314,7 +18155,9 @@
       <c r="E128" s="15">
         <v>560</v>
       </c>
-      <c r="F128" s="15"/>
+      <c r="F128" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="15">
       <c r="A129" s="15">
@@ -18332,7 +18175,9 @@
       <c r="E129" s="15">
         <v>560</v>
       </c>
-      <c r="F129" s="15"/>
+      <c r="F129" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="130" spans="1:6" ht="15">
       <c r="A130" s="15">
@@ -18350,7 +18195,9 @@
       <c r="E130" s="15">
         <v>560</v>
       </c>
-      <c r="F130" s="15"/>
+      <c r="F130" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="131" spans="1:6" ht="15">
       <c r="A131" s="15">
@@ -18368,7 +18215,9 @@
       <c r="E131" s="15">
         <v>560</v>
       </c>
-      <c r="F131" s="15"/>
+      <c r="F131" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="132" spans="1:6" ht="15">
       <c r="A132" s="15">
@@ -18384,7 +18233,9 @@
         <v>0</v>
       </c>
       <c r="E132" s="15"/>
-      <c r="F132" s="15"/>
+      <c r="F132" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="133" spans="1:6" ht="15">
       <c r="A133" s="15">
@@ -18402,7 +18253,9 @@
       <c r="E133" s="15">
         <v>560</v>
       </c>
-      <c r="F133" s="15"/>
+      <c r="F133" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="134" spans="1:6" ht="15">
       <c r="A134" s="15">
@@ -18418,7 +18271,9 @@
         <v>0</v>
       </c>
       <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
+      <c r="F134" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="135" spans="1:6" ht="15">
       <c r="A135" s="15">
@@ -18436,7 +18291,9 @@
       <c r="E135" s="15">
         <v>560</v>
       </c>
-      <c r="F135" s="15"/>
+      <c r="F135" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="15">
       <c r="A136" s="15">
@@ -18454,7 +18311,9 @@
       <c r="E136" s="15">
         <v>560</v>
       </c>
-      <c r="F136" s="15"/>
+      <c r="F136" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="137" spans="1:6" ht="15">
       <c r="A137" s="15">
@@ -18472,7 +18331,9 @@
       <c r="E137" s="15">
         <v>560</v>
       </c>
-      <c r="F137" s="15"/>
+      <c r="F137" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="138" spans="1:6" ht="15">
       <c r="A138" s="15">
@@ -18488,7 +18349,9 @@
         <v>0</v>
       </c>
       <c r="E138" s="15"/>
-      <c r="F138" s="15"/>
+      <c r="F138" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="139" spans="1:6" ht="15">
       <c r="A139" s="15">
@@ -18506,7 +18369,9 @@
       <c r="E139" s="15">
         <v>560</v>
       </c>
-      <c r="F139" s="15"/>
+      <c r="F139" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="140" spans="1:6" ht="15">
       <c r="A140" s="15">
@@ -18522,7 +18387,9 @@
         <v>0</v>
       </c>
       <c r="E140" s="15"/>
-      <c r="F140" s="15"/>
+      <c r="F140" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="141" spans="1:6" ht="15">
       <c r="A141" s="15">
@@ -18538,7 +18405,9 @@
         <v>0</v>
       </c>
       <c r="E141" s="15"/>
-      <c r="F141" s="15"/>
+      <c r="F141" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="142" spans="1:6" ht="15">
       <c r="A142" s="15">
@@ -18556,7 +18425,9 @@
       <c r="E142" s="15">
         <v>560</v>
       </c>
-      <c r="F142" s="15"/>
+      <c r="F142" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="143" spans="1:6" ht="15">
       <c r="A143" s="15">
@@ -18574,7 +18445,9 @@
       <c r="E143" s="15">
         <v>560</v>
       </c>
-      <c r="F143" s="15"/>
+      <c r="F143" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="144" spans="1:6" ht="15">
       <c r="A144" s="15">
@@ -18592,7 +18465,9 @@
       <c r="E144" s="15">
         <v>560</v>
       </c>
-      <c r="F144" s="15"/>
+      <c r="F144" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="145" spans="1:6" ht="15">
       <c r="A145" s="15">
@@ -18610,7 +18485,9 @@
       <c r="E145" s="15">
         <v>560</v>
       </c>
-      <c r="F145" s="15"/>
+      <c r="F145" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="146" spans="1:6" ht="15">
       <c r="A146" s="15">
@@ -18628,7 +18505,9 @@
       <c r="E146" s="15">
         <v>560</v>
       </c>
-      <c r="F146" s="15"/>
+      <c r="F146" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="147" spans="1:6" ht="15">
       <c r="A147" s="15">
@@ -18646,7 +18525,9 @@
       <c r="E147" s="15">
         <v>560</v>
       </c>
-      <c r="F147" s="15"/>
+      <c r="F147" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="148" spans="1:6" ht="15">
       <c r="A148" s="15">
@@ -18664,7 +18545,9 @@
       <c r="E148" s="15">
         <v>560</v>
       </c>
-      <c r="F148" s="15"/>
+      <c r="F148" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="149" spans="1:6" ht="15">
       <c r="A149" s="15">
@@ -18682,7 +18565,9 @@
       <c r="E149" s="15">
         <v>560</v>
       </c>
-      <c r="F149" s="15"/>
+      <c r="F149" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="150" spans="1:6" ht="15">
       <c r="A150" s="15">
@@ -18700,7 +18585,9 @@
       <c r="E150" s="15">
         <v>560</v>
       </c>
-      <c r="F150" s="15"/>
+      <c r="F150" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="151" spans="1:6" ht="15">
       <c r="A151" s="15">
@@ -18716,7 +18603,9 @@
         <v>0</v>
       </c>
       <c r="E151" s="15"/>
-      <c r="F151" s="15"/>
+      <c r="F151" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="152" spans="1:6" ht="15">
       <c r="A152" s="15">
@@ -18732,7 +18621,9 @@
         <v>0</v>
       </c>
       <c r="E152" s="15"/>
-      <c r="F152" s="15"/>
+      <c r="F152" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="153" spans="1:6" ht="15">
       <c r="A153" s="15">
@@ -18750,7 +18641,9 @@
       <c r="E153" s="15">
         <v>560</v>
       </c>
-      <c r="F153" s="15"/>
+      <c r="F153" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="154" spans="1:6" ht="15">
       <c r="A154" s="15">
@@ -18768,7 +18661,9 @@
       <c r="E154" s="15">
         <v>560</v>
       </c>
-      <c r="F154" s="15"/>
+      <c r="F154" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="155" spans="1:6" ht="15">
       <c r="A155" s="15">
@@ -18786,7 +18681,9 @@
       <c r="E155" s="15">
         <v>560</v>
       </c>
-      <c r="F155" s="15"/>
+      <c r="F155" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="156" spans="1:6" ht="15">
       <c r="A156" s="15">
@@ -18804,7 +18701,9 @@
       <c r="E156" s="15">
         <v>560</v>
       </c>
-      <c r="F156" s="15"/>
+      <c r="F156" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="157" spans="1:6" ht="15">
       <c r="A157" s="15">
@@ -18822,7 +18721,9 @@
       <c r="E157" s="15">
         <v>560</v>
       </c>
-      <c r="F157" s="15"/>
+      <c r="F157" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="158" spans="1:6" ht="15">
       <c r="A158" s="15">
@@ -18838,7 +18739,9 @@
         <v>0</v>
       </c>
       <c r="E158" s="15"/>
-      <c r="F158" s="15"/>
+      <c r="F158" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="159" spans="1:6" ht="15">
       <c r="A159" s="15">
@@ -18856,7 +18759,9 @@
       <c r="E159" s="15">
         <v>560</v>
       </c>
-      <c r="F159" s="15"/>
+      <c r="F159" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="160" spans="1:6" ht="15">
       <c r="A160" s="15">
@@ -18874,7 +18779,9 @@
       <c r="E160" s="15">
         <v>560</v>
       </c>
-      <c r="F160" s="15"/>
+      <c r="F160" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="161" spans="1:6" ht="15">
       <c r="A161" s="15">
@@ -18890,7 +18797,9 @@
         <v>0</v>
       </c>
       <c r="E161" s="15"/>
-      <c r="F161" s="15"/>
+      <c r="F161" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="162" spans="1:6" ht="15">
       <c r="A162" s="15">
@@ -18908,7 +18817,9 @@
       <c r="E162" s="15">
         <v>560</v>
       </c>
-      <c r="F162" s="15"/>
+      <c r="F162" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="163" spans="1:6" ht="15">
       <c r="A163" s="15">
@@ -18926,7 +18837,9 @@
       <c r="E163" s="15">
         <v>560</v>
       </c>
-      <c r="F163" s="15"/>
+      <c r="F163" s="15">
+        <v>43106</v>
+      </c>
     </row>
     <row r="164" spans="1:6" ht="15">
       <c r="A164" s="15">
@@ -18944,7 +18857,9 @@
       <c r="E164" s="15">
         <v>560</v>
       </c>
-      <c r="F164" s="15"/>
+      <c r="F164" s="15">
+        <v>43106</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -18954,10 +18869,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F187"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J187" sqref="J187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -22021,7 +21936,9 @@
       <c r="E153" s="7">
         <v>577</v>
       </c>
-      <c r="F153" s="7"/>
+      <c r="F153" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="154" spans="1:6" ht="16.5">
       <c r="A154" s="7">
@@ -22039,7 +21956,9 @@
       <c r="E154" s="7">
         <v>577</v>
       </c>
-      <c r="F154" s="7"/>
+      <c r="F154" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="155" spans="1:6" ht="28.5">
       <c r="A155" s="7">
@@ -22057,7 +21976,9 @@
       <c r="E155" s="7">
         <v>577</v>
       </c>
-      <c r="F155" s="7"/>
+      <c r="F155" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="156" spans="1:6" ht="28.5">
       <c r="A156" s="7">
@@ -22075,7 +21996,9 @@
       <c r="E156" s="7">
         <v>577</v>
       </c>
-      <c r="F156" s="7"/>
+      <c r="F156" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="157" spans="1:6" ht="16.5">
       <c r="A157" s="7">
@@ -22093,7 +22016,9 @@
       <c r="E157" s="7">
         <v>577</v>
       </c>
-      <c r="F157" s="7"/>
+      <c r="F157" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="158" spans="1:6" ht="28.5">
       <c r="A158" s="7">
@@ -22111,7 +22036,9 @@
       <c r="E158" s="7">
         <v>577</v>
       </c>
-      <c r="F158" s="7"/>
+      <c r="F158" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="159" spans="1:6" ht="28.5">
       <c r="A159" s="7">
@@ -22127,7 +22054,9 @@
         <v>0</v>
       </c>
       <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
+      <c r="F159" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="160" spans="1:6" ht="28.5">
       <c r="A160" s="7">
@@ -22145,7 +22074,9 @@
       <c r="E160" s="7">
         <v>577</v>
       </c>
-      <c r="F160" s="7"/>
+      <c r="F160" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="161" spans="1:6" ht="16.5">
       <c r="A161" s="7">
@@ -22163,7 +22094,9 @@
       <c r="E161" s="7">
         <v>577</v>
       </c>
-      <c r="F161" s="7"/>
+      <c r="F161" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="162" spans="1:6" ht="28.5">
       <c r="A162" s="7">
@@ -22179,7 +22112,9 @@
         <v>0</v>
       </c>
       <c r="E162" s="7"/>
-      <c r="F162" s="7"/>
+      <c r="F162" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="163" spans="1:6" ht="28.5">
       <c r="A163" s="7">
@@ -22197,7 +22132,9 @@
       <c r="E163" s="7">
         <v>577</v>
       </c>
-      <c r="F163" s="7"/>
+      <c r="F163" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="164" spans="1:6" ht="28.5">
       <c r="A164" s="7">
@@ -22215,7 +22152,9 @@
       <c r="E164" s="7">
         <v>577</v>
       </c>
-      <c r="F164" s="7"/>
+      <c r="F164" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="165" spans="1:6" ht="28.5">
       <c r="A165" s="7">
@@ -22233,7 +22172,9 @@
       <c r="E165" s="7">
         <v>577</v>
       </c>
-      <c r="F165" s="7"/>
+      <c r="F165" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="166" spans="1:6" ht="28.5">
       <c r="A166" s="7">
@@ -22251,7 +22192,9 @@
       <c r="E166" s="7">
         <v>577</v>
       </c>
-      <c r="F166" s="7"/>
+      <c r="F166" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="167" spans="1:6" ht="28.5">
       <c r="A167" s="7">
@@ -22269,7 +22212,9 @@
       <c r="E167" s="7">
         <v>577</v>
       </c>
-      <c r="F167" s="7"/>
+      <c r="F167" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="168" spans="1:6" ht="28.5">
       <c r="A168" s="7">
@@ -22287,7 +22232,9 @@
       <c r="E168" s="7">
         <v>577</v>
       </c>
-      <c r="F168" s="7"/>
+      <c r="F168" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="169" spans="1:6" ht="28.5">
       <c r="A169" s="7">
@@ -22305,7 +22252,9 @@
       <c r="E169" s="7">
         <v>577</v>
       </c>
-      <c r="F169" s="7"/>
+      <c r="F169" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="170" spans="1:6" ht="28.5">
       <c r="A170" s="7">
@@ -22323,7 +22272,9 @@
       <c r="E170" s="7">
         <v>577</v>
       </c>
-      <c r="F170" s="7"/>
+      <c r="F170" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="171" spans="1:6" ht="16.5">
       <c r="A171" s="7">
@@ -22341,7 +22292,9 @@
       <c r="E171" s="7">
         <v>577</v>
       </c>
-      <c r="F171" s="7"/>
+      <c r="F171" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="172" spans="1:6" ht="16.5">
       <c r="A172" s="7">
@@ -22359,7 +22312,9 @@
       <c r="E172" s="7">
         <v>577</v>
       </c>
-      <c r="F172" s="7"/>
+      <c r="F172" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="173" spans="1:6" ht="28.5">
       <c r="A173" s="7">
@@ -22377,7 +22332,9 @@
       <c r="E173" s="7">
         <v>577</v>
       </c>
-      <c r="F173" s="7"/>
+      <c r="F173" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="174" spans="1:6" ht="28.5">
       <c r="A174" s="7">
@@ -22395,7 +22352,9 @@
       <c r="E174" s="7">
         <v>577</v>
       </c>
-      <c r="F174" s="7"/>
+      <c r="F174" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="175" spans="1:6" ht="28.5">
       <c r="A175" s="7">
@@ -22413,7 +22372,9 @@
       <c r="E175" s="7">
         <v>577</v>
       </c>
-      <c r="F175" s="7"/>
+      <c r="F175" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="176" spans="1:6" ht="28.5">
       <c r="A176" s="7">
@@ -22431,7 +22392,9 @@
       <c r="E176" s="7">
         <v>577</v>
       </c>
-      <c r="F176" s="7"/>
+      <c r="F176" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="177" spans="1:6" ht="16.5">
       <c r="A177" s="7">
@@ -22449,7 +22412,9 @@
       <c r="E177" s="7">
         <v>577</v>
       </c>
-      <c r="F177" s="7"/>
+      <c r="F177" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="178" spans="1:6" ht="28.5">
       <c r="A178" s="7">
@@ -22467,7 +22432,9 @@
       <c r="E178" s="7">
         <v>577</v>
       </c>
-      <c r="F178" s="7"/>
+      <c r="F178" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="179" spans="1:6" ht="28.5">
       <c r="A179" s="7">
@@ -22485,7 +22452,9 @@
       <c r="E179" s="7">
         <v>577</v>
       </c>
-      <c r="F179" s="7"/>
+      <c r="F179" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="180" spans="1:6" ht="28.5">
       <c r="A180" s="7">
@@ -22503,7 +22472,9 @@
       <c r="E180" s="7">
         <v>577</v>
       </c>
-      <c r="F180" s="7"/>
+      <c r="F180" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="181" spans="1:6" ht="28.5">
       <c r="A181" s="7">
@@ -22521,7 +22492,9 @@
       <c r="E181" s="7">
         <v>577</v>
       </c>
-      <c r="F181" s="7"/>
+      <c r="F181" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="182" spans="1:6" ht="28.5">
       <c r="A182" s="7">
@@ -22539,7 +22512,9 @@
       <c r="E182" s="7">
         <v>577</v>
       </c>
-      <c r="F182" s="7"/>
+      <c r="F182" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="183" spans="1:6" ht="28.5">
       <c r="A183" s="7">
@@ -22557,7 +22532,9 @@
       <c r="E183" s="7">
         <v>577</v>
       </c>
-      <c r="F183" s="7"/>
+      <c r="F183" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="184" spans="1:6" ht="47.25">
       <c r="A184" s="7">
@@ -22575,7 +22552,9 @@
       <c r="E184" s="7">
         <v>577</v>
       </c>
-      <c r="F184" s="7"/>
+      <c r="F184" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="185" spans="1:6" ht="47.25">
       <c r="A185" s="7">
@@ -22593,7 +22572,9 @@
       <c r="E185" s="7">
         <v>577</v>
       </c>
-      <c r="F185" s="7"/>
+      <c r="F185" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="186" spans="1:6" ht="61.5">
       <c r="A186" s="7">
@@ -22611,7 +22592,9 @@
       <c r="E186" s="7">
         <v>577</v>
       </c>
-      <c r="F186" s="7"/>
+      <c r="F186" s="7">
+        <v>51000</v>
+      </c>
     </row>
     <row r="187" spans="1:6" ht="61.5">
       <c r="A187" s="7">
@@ -22629,7 +22612,12 @@
       <c r="E187" s="7">
         <v>577</v>
       </c>
-      <c r="F187" s="7"/>
+      <c r="F187" s="7">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="16.5">
+      <c r="F188" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
delete the university with wrong location
</commit_message>
<xml_diff>
--- a/ScienceAdmissionScore.xlsx
+++ b/ScienceAdmissionScore.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xuhao.du.UWA\Peter Du\University entrance exam\Chinese_University_Entrance_Ranking_GD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xuhao.du.UWA\Peter Du\University entrance exam\Chinese_University_Entrance_Ranking_GD\Chinese_University_Entrance_Ranking_GD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="456"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="2014" sheetId="5" r:id="rId5"/>
     <sheet name="2015" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="379">
   <si>
     <t>院校号</t>
   </si>
@@ -2986,10 +2986,16 @@
     </r>
   </si>
   <si>
-    <t>汕头大学（汕头大学医）</t>
-  </si>
-  <si>
-    <t>汕头大学（汕头大学医学）</t>
+    <t>上海交通大学医学</t>
+  </si>
+  <si>
+    <t>复旦大学医学</t>
+  </si>
+  <si>
+    <t>浙江大学医学</t>
+  </si>
+  <si>
+    <t>汕头大学(汕头大学医学)</t>
   </si>
   <si>
     <r>
@@ -3012,7 +3018,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>汕头大学医</t>
+      <t>汕头大学医学</t>
     </r>
     <r>
       <rPr>
@@ -3046,7 +3052,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>汕头大学医</t>
+      <t>汕头大学医学</t>
     </r>
     <r>
       <rPr>
@@ -3058,18 +3064,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>上海交通大学医学</t>
-  </si>
-  <si>
-    <t>复旦大学医学</t>
-  </si>
-  <si>
-    <t>上海交通大学医</t>
-  </si>
-  <si>
-    <t>浙江大学医学</t>
   </si>
 </sst>
 </file>
@@ -3577,8 +3571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5953,7 +5947,7 @@
         <v>240</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C119" s="2">
         <v>246</v>
@@ -6379,7 +6373,7 @@
   <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6634,7 +6628,7 @@
         <v>19248</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C13" s="4">
         <v>8</v>
@@ -7914,7 +7908,7 @@
         <v>80001</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C77" s="4">
         <v>246</v>
@@ -9259,8 +9253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9475,7 +9469,7 @@
         <v>19248</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C11" s="5">
         <v>8</v>
@@ -11035,7 +11029,7 @@
         <v>80001</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C89" s="5">
         <v>242</v>
@@ -12200,8 +12194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12336,7 +12330,7 @@
         <v>19248</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C7" s="12">
         <v>8</v>
@@ -12376,7 +12370,7 @@
         <v>19246</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C9" s="12">
         <v>15</v>
@@ -13351,12 +13345,12 @@
         <v>17854</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30">
+    <row r="58" spans="1:6" ht="15">
       <c r="A58" s="11">
         <v>80001</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C58" s="12">
         <v>242</v>
@@ -15282,7 +15276,7 @@
   <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E161" sqref="E161"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15497,7 +15491,7 @@
         <v>19246</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C11" s="15">
         <v>11</v>
@@ -15597,7 +15591,7 @@
         <v>19248</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C16" s="15">
         <v>7</v>
@@ -16177,7 +16171,7 @@
         <v>80001</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C45" s="15">
         <v>242</v>
@@ -18582,8 +18576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H159" sqref="H159"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18698,7 +18692,7 @@
         <v>19248</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -18718,7 +18712,7 @@
         <v>19246</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
@@ -19098,7 +19092,7 @@
         <v>19335</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C26" s="7">
         <v>20</v>
@@ -20438,7 +20432,7 @@
         <v>80001</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C93" s="7">
         <v>240</v>

</xml_diff>